<commit_message>
Update OOP sample final tests
</commit_message>
<xml_diff>
--- a/IT002-OOP/it002m21mmcl/it002m21mmcl1.xlsx
+++ b/IT002-OOP/it002m21mmcl/it002m21mmcl1.xlsx
@@ -481,7 +481,9 @@
       <c r="E2" t="n">
         <v>800</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>500</v>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -503,7 +505,9 @@
       <c r="E3" t="n">
         <v>600</v>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>500</v>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
     </row>
@@ -545,7 +549,9 @@
       <c r="E5" t="n">
         <v>600</v>
       </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>500</v>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
     </row>
@@ -565,7 +571,9 @@
         <v>600</v>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>800</v>
+      </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
     </row>
@@ -585,7 +593,9 @@
         <v>600</v>
       </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>300</v>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
     </row>
@@ -601,7 +611,9 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>300</v>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
     </row>
@@ -623,7 +635,9 @@
       <c r="E9" t="n">
         <v>400</v>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>400</v>
+      </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
     </row>
@@ -645,7 +659,9 @@
       <c r="E10" t="n">
         <v>800</v>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>800</v>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
     </row>
@@ -665,7 +681,9 @@
       <c r="E11" t="n">
         <v>800</v>
       </c>
-      <c r="F11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>800</v>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
     </row>
@@ -685,7 +703,9 @@
       <c r="E12" t="n">
         <v>300</v>
       </c>
-      <c r="F12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>800</v>
+      </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
     </row>
@@ -707,7 +727,9 @@
       <c r="E13" t="n">
         <v>500</v>
       </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>800</v>
+      </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
     </row>
@@ -729,7 +751,9 @@
       <c r="E14" t="n">
         <v>600</v>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>400</v>
+      </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
     </row>
@@ -751,7 +775,9 @@
       <c r="E15" t="n">
         <v>700</v>
       </c>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>800</v>
+      </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
     </row>
@@ -773,7 +799,9 @@
       <c r="E16" t="n">
         <v>600</v>
       </c>
-      <c r="F16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>400</v>
+      </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
     </row>
@@ -813,7 +841,9 @@
       <c r="E18" t="n">
         <v>750</v>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>800</v>
+      </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
     </row>
@@ -853,7 +883,9 @@
       <c r="E20" t="n">
         <v>600</v>
       </c>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>800</v>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
     </row>
@@ -875,7 +907,9 @@
       <c r="E21" t="n">
         <v>700</v>
       </c>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>300</v>
+      </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
     </row>

</xml_diff>